<commit_message>
corrected input variable and stats function for {tx|tn|tm}{min|max|mean}
</commit_message>
<xml_diff>
--- a/climate_indices_CV21.xlsx
+++ b/climate_indices_CV21.xlsx
@@ -23,55 +23,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <authors>
-    <author> </author>
-  </authors>
-  <commentList>
-    <comment ref="B30" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Note that ETCCDI and ET-SCI "defines" daily mean temperature as the average of Tmax and Tmin (CF cell method "mid_range"). In model comparisons this is often relaxed (overlooked),  and instead uses daily data based on whatever time step or output/sampling frequency was used to produce it.</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <authors>
-    <author> </author>
-  </authors>
-  <commentList>
-    <comment ref="B1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Included – or not in the main table:
-0 – not
-1 – doable
-2 – done</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2939,7 +2890,7 @@
     <numFmt numFmtId="166" formatCode="#,##0"/>
     <numFmt numFmtId="167" formatCode="@"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -3070,6 +3021,12 @@
       <color rgb="FF800000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="6.4"/>
+      <color rgb="FF000000"/>
+      <name val="Cantarell"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="9">
@@ -3735,6 +3692,459 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
 </file>
 
+<file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" guid="{3D3F5988-65AE-496C-A237-39963F136672}">
+  <header guid="{503739F5-5264-47C6-8E6A-4C189FBD0B49}" dateTime="2019-05-20T15:22:00.000000000Z" userName=" " r:id="rId1" minRId="1" maxRId="9" maxSheetId="4">
+    <sheetIdMap count="3">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{3D3F5988-65AE-496C-A237-39963F136672}" dateTime="2019-05-20T15:23:00.000000000Z" userName=" " r:id="rId2" minRId="10" maxRId="15" maxSheetId="4">
+    <sheetIdMap count="3">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+    </sheetIdMap>
+  </header>
+</headers>
+</file>
+
+<file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="1" ua="true" sId="1">
+    <oc r="A38" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="6.4"/>
+            <color rgb="FF000000"/>
+            <rFont val="Cantarell"/>
+            <family val="0"/>
+          </rPr>
+          <t xml:space="preserve">    ----  {variable}{comparison_operator}{threshold_value}</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="A38" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">ctmle#</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="2" ua="false" sId="1">
+    <oc r="AB48" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">time: maximum</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AB48" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">time: minimum</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="3" ua="false" sId="1">
+    <oc r="Y49" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">tasmax</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="Y49" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">tas</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="4" ua="false" sId="1">
+    <oc r="AB49" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">time: minimum</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AB49" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">time: mean</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="5" ua="false" sId="1">
+    <oc r="Y50" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">tasmin</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="Y50" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">tas</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="6" ua="false" sId="1">
+    <oc r="AB50" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">time: minimum</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AB50" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">time: mean</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="7" ua="false" sId="1">
+    <oc r="AB51" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">time: mean</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AB51" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">time: maximum</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="8" ua="false" sId="1">
+    <oc r="AB52" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">time: mean</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AB52" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">time: minimum</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="9" ua="true" sId="1">
+    <oc r="AB48" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">time: minimum</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AB48" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">time: maximum</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="10" ua="true" sId="1">
+    <oc r="Y49" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">tas</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="Y49" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">tasmax</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="11" ua="true" sId="1">
+    <oc r="AB49" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">time: mean</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AB49" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">time: minimum</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="12" ua="true" sId="1">
+    <oc r="Y50" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">tas</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="Y50" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">tasmin</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="13" ua="true" sId="1">
+    <oc r="AB50" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">time: mean</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AB50" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">time: minimum</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="14" ua="true" sId="1">
+    <oc r="AB51" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">time: maximum</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AB51" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">time: mean</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="15" ua="true" sId="1">
+    <oc r="AB52" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">time: minimum</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="AB52" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">time: mean</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="0"/>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
@@ -3743,11 +4153,11 @@
   <dimension ref="A1:AP126"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="X9" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="X1" activeCellId="0" sqref="X1"/>
+      <selection pane="bottomLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+      <selection pane="bottomRight" activeCell="AB52" activeCellId="0" sqref="AB52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8901,7 +9311,7 @@
         <v>46</v>
       </c>
       <c r="AB48" s="44" t="s">
-        <v>51</v>
+        <v>82</v>
       </c>
       <c r="AC48" s="38" t="s">
         <v>156</v>
@@ -8998,7 +9408,7 @@
         <v>156</v>
       </c>
       <c r="Y49" s="44" t="s">
-        <v>122</v>
+        <v>81</v>
       </c>
       <c r="Z49" s="44" t="s">
         <v>50</v>
@@ -9007,7 +9417,7 @@
         <v>46</v>
       </c>
       <c r="AB49" s="44" t="s">
-        <v>123</v>
+        <v>51</v>
       </c>
       <c r="AC49" s="38" t="s">
         <v>156</v>
@@ -9104,7 +9514,7 @@
         <v>156</v>
       </c>
       <c r="Y50" s="44" t="s">
-        <v>122</v>
+        <v>49</v>
       </c>
       <c r="Z50" s="44" t="s">
         <v>50</v>
@@ -9113,7 +9523,7 @@
         <v>46</v>
       </c>
       <c r="AB50" s="44" t="s">
-        <v>123</v>
+        <v>51</v>
       </c>
       <c r="AC50" s="38" t="s">
         <v>156</v>
@@ -9219,7 +9629,7 @@
         <v>46</v>
       </c>
       <c r="AB51" s="44" t="s">
-        <v>82</v>
+        <v>123</v>
       </c>
       <c r="AC51" s="38" t="s">
         <v>156</v>
@@ -9325,7 +9735,7 @@
         <v>46</v>
       </c>
       <c r="AB52" s="44" t="s">
-        <v>51</v>
+        <v>123</v>
       </c>
       <c r="AC52" s="38" t="s">
         <v>156</v>
@@ -17592,7 +18002,6 @@
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -18659,6 +19068,5 @@
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>